<commit_message>
Added new "straight" report type - shows data as it is without aggregation
..and fixed wrong logsSource representation in UI
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -245,19 +245,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <b val="true"/>
@@ -543,13 +540,13 @@
   </sheetPr>
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z8" activeCellId="0" sqref="Z8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -944,8 +941,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reordered (renamed) 3 columns in template
Looks like data was populated in wrong columns..?
T Жидкости/Газа/Теплоносителя --> T Теплоносителя/Жидкости/Газа
ТТ008/ТТ007/ТТ009 --> ТТ007/ТТ009/ТТ008
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -123,15 +123,15 @@
     <t xml:space="preserve">Плотность</t>
   </si>
   <si>
+    <t xml:space="preserve">Т. Теплоносителя</t>
+  </si>
+  <si>
     <t xml:space="preserve">Т. жидкости</t>
   </si>
   <si>
     <t xml:space="preserve">Т. газа</t>
   </si>
   <si>
-    <t xml:space="preserve">Т. Теплоносителя</t>
-  </si>
-  <si>
     <t xml:space="preserve">РТ001</t>
   </si>
   <si>
@@ -186,13 +186,13 @@
     <t xml:space="preserve">PT008</t>
   </si>
   <si>
+    <t xml:space="preserve">TT007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT009</t>
+  </si>
+  <si>
     <t xml:space="preserve">TT008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TT007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TT009</t>
   </si>
   <si>
     <t xml:space="preserve">МПа</t>
@@ -543,13 +543,14 @@
   </sheetPr>
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG5" activeCellId="0" sqref="AG5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>